<commit_message>
update ANP Hamburger model
</commit_message>
<xml_diff>
--- a/Examples/ANP_Hamburger_Marketshare/HamburgerModel_Excel_filledIn.xlsx
+++ b/Examples/ANP_Hamburger_Marketshare/HamburgerModel_Excel_filledIn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/GITHUB/AhpAnpLib/Examples/ANP_Hamburger_Marketshare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97460FBB-810F-9748-81B8-7FCE7670D193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730E701C-32E1-A242-9DC3-3A1FA8B01C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="20780" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="23">
   <si>
     <t>1 McDonald's</t>
-  </si>
-  <si>
-    <t>Enter judgments for the paiwise comparisons in the matrix or direct values in the green cells</t>
   </si>
   <si>
     <t>1 Alternatives</t>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>8 Reputation</t>
+  </si>
+  <si>
+    <t>Enter pairwise comparisons in the white cells of the table or numerical data in the green cells. For the Direct Values column, if the smallest value is best, invert the value before entering it (e.g., $10 as =1/10) .</t>
   </si>
 </sst>
 </file>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
-      <selection activeCell="B351" sqref="B351:J360"/>
+    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
+      <selection activeCell="A339" sqref="A339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -572,26 +572,26 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>1</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="8">
         <f>1/C4</f>
@@ -616,29 +616,29 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="8">
         <f>1/C10</f>
@@ -671,7 +671,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="8">
         <f>1/D10</f>
@@ -688,29 +688,29 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="8">
         <f>1/C17</f>
@@ -743,7 +743,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="8">
         <f>1/D17</f>
@@ -760,44 +760,44 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="J23" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="8">
         <f>1/C24</f>
@@ -865,7 +865,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="8">
         <f>1/D24</f>
@@ -901,7 +901,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="8">
         <f>1/E24</f>
@@ -937,7 +937,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="8">
         <f>1/F24</f>
@@ -972,7 +972,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="8">
         <f>1/G24</f>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="8">
         <f>1/H24</f>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" s="8">
         <f>1/I24</f>
@@ -1080,26 +1080,26 @@
     </row>
     <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1116,7 +1116,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B38" s="8">
         <f>1/C37</f>
@@ -1129,29 +1129,29 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E42" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" s="8" t="e">
         <f>1/C39</f>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" s="8">
         <f>1/D43</f>
@@ -1199,29 +1199,29 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E49" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="5">
         <v>1</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51" s="8">
         <f>1/C50</f>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" s="8">
         <f>1/D50</f>
@@ -1269,44 +1269,44 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="E56" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="F56" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="G56" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G56" s="4" t="s">
+      <c r="H56" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="4" t="s">
+      <c r="I56" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I56" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="J56" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B57" s="5">
         <v>1</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B58" s="8">
         <f>1/C57</f>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" s="8">
         <f>1/D57</f>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B60" s="8">
         <f>1/E57</f>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B61" s="8">
         <f>1/F57</f>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B62" s="8">
         <f>1/G57</f>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B63" s="8">
         <f>1/H57</f>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B64" s="8">
         <f>1/I57</f>
@@ -1574,26 +1574,26 @@
     </row>
     <row r="67" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -1610,7 +1610,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B71" s="8">
         <f>1/C70</f>
@@ -1623,29 +1623,29 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="D75" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E75" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B76" s="5">
         <v>1</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B77" s="8">
         <f>1/C76</f>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B78" s="8">
         <f>1/D76</f>
@@ -1693,29 +1693,29 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="C82" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="D82" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E82" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B83" s="5">
         <v>1</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B84" s="8">
         <f>1/C83</f>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B85" s="8">
         <f>1/D83</f>
@@ -1763,44 +1763,44 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="C89" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="D89" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="E89" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="F89" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="G89" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="H89" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H89" s="4" t="s">
+      <c r="I89" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I89" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="J89" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B90" s="5">
         <v>1</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B91" s="8">
         <f>1/C90</f>
@@ -1861,7 +1861,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B92" s="8">
         <f>1/D90</f>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B93" s="8">
         <f>1/E90</f>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B94" s="8">
         <f>1/F90</f>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B95" s="8">
         <f>1/G90</f>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B96" s="8">
         <f>1/H90</f>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B97" s="8">
         <f>1/I90</f>
@@ -2068,29 +2068,29 @@
     </row>
     <row r="100" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C102" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E102" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
@@ -2110,7 +2110,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B104" s="8">
         <f>1/C103</f>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B105" s="8">
         <f>1/D103</f>
@@ -2143,26 +2143,26 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B109" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C109" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D109" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B110" s="5">
         <v>1</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B111" s="8">
         <f>1/C110</f>
@@ -2188,29 +2188,29 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B116" s="5">
         <v>1</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B117" s="8">
         <f>1/C116</f>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B118" s="8">
         <f>1/D116</f>
@@ -2259,29 +2259,29 @@
     </row>
     <row r="121" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C123" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D123" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D123" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E123" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -2301,7 +2301,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B125" s="8">
         <f>1/C124</f>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B126" s="8">
         <f>1/D124</f>
@@ -2334,26 +2334,26 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C130" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D130" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B131" s="5">
         <v>1</v>
@@ -2365,7 +2365,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B132" s="8">
         <f>1/C131</f>
@@ -2378,26 +2378,26 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B136" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B136" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="C136" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B137" s="5">
         <v>1</v>
@@ -2409,7 +2409,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B138" s="8">
         <f>1/C137</f>
@@ -2422,29 +2422,29 @@
     </row>
     <row r="141" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C143" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D143" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D143" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E143" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -2464,7 +2464,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B145" s="8">
         <f>1/C144</f>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B146" s="8">
         <f>1/D144</f>
@@ -2497,26 +2497,26 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B150" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="C150" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C150" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="D150" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B151" s="5">
         <v>1</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B152" s="8">
         <f>1/C151</f>
@@ -2541,29 +2541,29 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B157" s="5">
         <v>1</v>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B158" s="8">
         <f>1/C157</f>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B159" s="8">
         <f>1/D157</f>
@@ -2611,29 +2611,29 @@
     </row>
     <row r="162" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C164" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D164" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D164" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E164" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -2653,7 +2653,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B166" s="8">
         <f>1/C165</f>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B167" s="8">
         <f>1/D165</f>
@@ -2686,29 +2686,29 @@
     </row>
     <row r="170" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B172" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C172" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D172" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D172" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E172" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -2728,7 +2728,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B174" s="8">
         <f>1/C173</f>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B175" s="8">
         <f>1/D173</f>
@@ -2761,29 +2761,29 @@
     </row>
     <row r="178" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B180" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C180" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D180" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D180" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E180" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -2803,7 +2803,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B182" s="8">
         <f>1/C181</f>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B183" s="8">
         <f>1/D181</f>
@@ -2836,26 +2836,26 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B187" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B187" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="C187" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D187" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B188" s="5">
         <v>1</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B189" s="8">
         <f>1/C188</f>
@@ -2880,29 +2880,29 @@
     </row>
     <row r="192" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B194" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C194" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D194" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D194" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E194" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -2922,7 +2922,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B196" s="8">
         <f>1/C195</f>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B197" s="8">
         <f>1/D195</f>
@@ -2955,26 +2955,26 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B201" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C201" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C201" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D201" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B202" s="5">
         <v>1</v>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B203" s="8">
         <f>1/C202</f>
@@ -2999,26 +2999,26 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B207" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B207" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="C207" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B208" s="5">
         <v>1</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B209" s="8">
         <f>1/C208</f>
@@ -3043,26 +3043,26 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B214" s="5">
         <v>1</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B215" s="8">
         <f>1/C214</f>
@@ -3087,29 +3087,29 @@
     </row>
     <row r="218" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B220" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C220" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D220" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D220" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E220" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
@@ -3129,7 +3129,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B222" s="8">
         <f>1/C221</f>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B223" s="8">
         <f>1/D221</f>
@@ -3162,29 +3162,29 @@
     </row>
     <row r="226" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B228" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C228" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D228" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D228" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E228" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
@@ -3204,7 +3204,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B230" s="8">
         <f>1/C229</f>
@@ -3220,7 +3220,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B231" s="8">
         <f>1/D229</f>
@@ -3237,32 +3237,32 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C235" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D235" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D235" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="E235" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F235" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B236" s="5">
         <v>1</v>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B237" s="8">
         <f>1/C236</f>
@@ -3299,7 +3299,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B238" s="8">
         <f>1/D236</f>
@@ -3319,7 +3319,7 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B239" s="8">
         <f>1/E236</f>
@@ -3340,29 +3340,29 @@
     </row>
     <row r="242" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B244" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C244" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D244" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D244" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E244" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
@@ -3382,7 +3382,7 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B246" s="8">
         <f>1/C245</f>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B247" s="8">
         <f>1/D245</f>
@@ -3415,29 +3415,29 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C251" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D251" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D251" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E251" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B252" s="5">
         <v>1</v>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B253" s="8">
         <f>1/C252</f>
@@ -3468,7 +3468,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B254" s="8">
         <f>1/D252</f>
@@ -3485,29 +3485,29 @@
     </row>
     <row r="257" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B259" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C259" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D259" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D259" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E259" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
@@ -3527,7 +3527,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B261" s="8">
         <f>1/C260</f>
@@ -3543,7 +3543,7 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B262" s="8">
         <f>1/D260</f>
@@ -3560,29 +3560,29 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B266" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C266" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C266" s="4" t="s">
+      <c r="D266" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D266" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="E266" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B267" s="5">
         <v>1</v>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B268" s="8">
         <f>1/C267</f>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B269" s="8">
         <f>1/D267</f>
@@ -3630,29 +3630,29 @@
     </row>
     <row r="272" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B274" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C274" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D274" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D274" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E274" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.2">
@@ -3672,7 +3672,7 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B276" s="8">
         <f>1/C275</f>
@@ -3688,7 +3688,7 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B277" s="8">
         <f>1/D275</f>
@@ -3705,29 +3705,29 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B281" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B281" s="4" t="s">
+      <c r="C281" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C281" s="4" t="s">
+      <c r="D281" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D281" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E281" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B282" s="5">
         <v>1</v>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B283" s="8">
         <f>1/C282</f>
@@ -3758,7 +3758,7 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B284" s="8">
         <f>1/D282</f>
@@ -3775,29 +3775,29 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B288" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B288" s="4" t="s">
+      <c r="C288" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C288" s="4" t="s">
+      <c r="D288" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D288" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E288" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B289" s="5">
         <v>1</v>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B290" s="8">
         <f>1/C289</f>
@@ -3828,7 +3828,7 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B291" s="8">
         <f>1/D289</f>
@@ -3845,32 +3845,32 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B295" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B295" s="4" t="s">
+      <c r="C295" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C295" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="D295" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E295" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E295" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="F295" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B296" s="5">
         <v>1</v>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B297" s="8">
         <f>1/C296</f>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B298" s="8">
         <f>1/D296</f>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B299" s="8">
         <f>1/E296</f>
@@ -3948,29 +3948,29 @@
     </row>
     <row r="302" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B304" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C304" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D304" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D304" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E304" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.2">
@@ -3990,7 +3990,7 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B306" s="8">
         <f>1/C305</f>
@@ -4006,7 +4006,7 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B307" s="8">
         <f>1/D305</f>
@@ -4023,29 +4023,29 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B311" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C311" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C311" s="4" t="s">
+      <c r="D311" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D311" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="E311" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B312" s="5">
         <v>1</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B313" s="8">
         <f>1/C312</f>
@@ -4077,7 +4077,7 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B314" s="8">
         <f>1/D312</f>
@@ -4094,29 +4094,29 @@
     </row>
     <row r="317" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B319" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C319" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D319" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D319" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E319" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.2">
@@ -4136,7 +4136,7 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B321" s="8">
         <f>1/C320</f>
@@ -4152,7 +4152,7 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B322" s="8">
         <f>1/D320</f>
@@ -4169,29 +4169,29 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B326" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B326" s="4" t="s">
+      <c r="C326" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C326" s="4" t="s">
+      <c r="D326" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D326" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E326" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B327" s="5">
         <v>1</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B328" s="8">
         <f>1/C327</f>
@@ -4222,7 +4222,7 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B329" s="8">
         <f>1/D327</f>
@@ -4239,29 +4239,29 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B333" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B333" s="4" t="s">
+      <c r="C333" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C333" s="4" t="s">
+      <c r="D333" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D333" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E333" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B334" s="5">
         <v>1</v>
@@ -4276,7 +4276,7 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B335" s="8">
         <f>1/C334</f>
@@ -4292,7 +4292,7 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B336" s="8">
         <f>1/D334</f>
@@ -4309,44 +4309,44 @@
     </row>
     <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B340" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B340" s="4" t="s">
+      <c r="C340" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C340" s="4" t="s">
+      <c r="D340" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D340" s="4" t="s">
+      <c r="E340" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E340" s="4" t="s">
+      <c r="F340" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F340" s="4" t="s">
+      <c r="G340" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G340" s="4" t="s">
+      <c r="H340" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H340" s="4" t="s">
+      <c r="I340" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I340" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="J340" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B341" s="5">
         <v>1</v>
@@ -4376,7 +4376,7 @@
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B342" s="8">
         <f>1/C341</f>
@@ -4407,7 +4407,7 @@
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B343" s="8">
         <f>1/D341</f>
@@ -4439,7 +4439,7 @@
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B344" s="8">
         <f>1/E341</f>
@@ -4472,7 +4472,7 @@
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A345" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B345" s="8">
         <f>1/F341</f>
@@ -4506,7 +4506,7 @@
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A346" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B346" s="8">
         <f>1/G341</f>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B347" s="8">
         <f>1/H341</f>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B348" s="8">
         <f>1/I341</f>

</xml_diff>